<commit_message>
SFT i Dodatkowa dokumentacja do X10
Dodano SFT Table oraz dodatkową dokumentację do
modułu X10. Teraz wiadomo jak to się podłącza
</commit_message>
<xml_diff>
--- a/PROTOKOŁY/USTERKI.xlsx
+++ b/PROTOKOŁY/USTERKI.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\PROJEKTY\2021\Hotel Europejski\SERWER\PROTOKOŁY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2697F582-1BFB-471E-B2D4-6DF1B44B4FF7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FDAA96E-1414-4FBD-9313-6D7E9F6E0019}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="LISTA" sheetId="1" r:id="rId1"/>
+    <sheet name="Aktualna Lista" sheetId="1" r:id="rId1"/>
     <sheet name="Tabela wejściwa" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="61">
   <si>
     <t>ID</t>
   </si>
@@ -203,6 +203,12 @@
   </si>
   <si>
     <t>Incomm</t>
+  </si>
+  <si>
+    <t>znalezione 3 pokoje (z 5 przeglądanych) gdzie stycznik K0 jest załączony pomimo braku obecności - wyłączone ze sprzedaży od długiego czasu. Światło załączone, podłoga grzeje bez sensu… Do inwentaryzacji wszystkie pokoje w celu wyłapania wszystkich pokoi z takim problemem</t>
+  </si>
+  <si>
+    <t>pomiar temperatury płaski jak od linijki - uszkodzenie nastawmika</t>
   </si>
 </sst>
 </file>
@@ -210,7 +216,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -383,63 +389,69 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -478,9 +490,6 @@
         </bottom>
       </border>
     </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -500,10 +509,10 @@
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{E800D0FF-9E5E-41DB-8A7E-12A96BA8D8D3}" name="ID"/>
     <tableColumn id="10" xr3:uid="{05B6C2FD-8E0C-47E3-8636-3220BB4FA4A6}" name="DATA WYKRYCIA"/>
-    <tableColumn id="11" xr3:uid="{34BE2DAC-1195-447A-8FD8-61A0B01F2F66}" name="WYKRYŁ" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{A3AFA416-3BCC-4DDB-9610-9503A0DBF1ED}" name="POKÓJ" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{FAA4DD45-A2AE-48A7-9914-D8B0D0C336E4}" name="TYP POKOJU"/>
-    <tableColumn id="4" xr3:uid="{B3ADF2B4-89C3-4637-9727-64DE12E835CA}" name="OPIS" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{34BE2DAC-1195-447A-8FD8-61A0B01F2F66}" name="WYKRYŁ" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{A3AFA416-3BCC-4DDB-9610-9503A0DBF1ED}" name="POKÓJ" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{FAA4DD45-A2AE-48A7-9914-D8B0D0C336E4}" name="TYP POKOJU" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{B3ADF2B4-89C3-4637-9727-64DE12E835CA}" name="OPIS" dataDxfId="1"/>
     <tableColumn id="5" xr3:uid="{17C531FF-04C8-41CD-9927-F558D42FC929}" name="ROZWIĄZANIE"/>
     <tableColumn id="6" xr3:uid="{63B39581-7931-464B-A124-3253D048810A}" name="DATA ROZWIZANIA"/>
     <tableColumn id="7" xr3:uid="{BA5CB0E0-DB7F-4DFF-BEB1-AFC08CB72022}" name="WYKONAŁ"/>
@@ -778,14 +787,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="4" width="22.85546875" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
     <col min="7" max="7" width="106.7109375" customWidth="1"/>
     <col min="8" max="8" width="79.28515625" customWidth="1"/>
@@ -833,16 +844,16 @@
       <c r="C3" s="1">
         <v>44273</v>
       </c>
-      <c r="D3" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="29">
+      <c r="D3" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="23">
         <v>305</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="28" t="s">
+      <c r="G3" s="22" t="s">
         <v>8</v>
       </c>
     </row>
@@ -853,16 +864,16 @@
       <c r="C4" s="1">
         <v>44273</v>
       </c>
-      <c r="D4" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="29">
+      <c r="D4" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="23">
         <v>305</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="28" t="s">
+      <c r="G4" s="22" t="s">
         <v>10</v>
       </c>
       <c r="H4" t="s">
@@ -879,36 +890,37 @@
       <c r="B5">
         <v>1671</v>
       </c>
-      <c r="C5" s="30">
+      <c r="C5" s="24">
         <v>43621</v>
       </c>
-      <c r="D5" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="29">
+      <c r="D5" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="23">
         <v>307</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="28" t="s">
+      <c r="G5" s="22" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>2607</v>
       </c>
-      <c r="C6" s="30">
+      <c r="C6" s="24">
         <v>43880</v>
       </c>
-      <c r="D6" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="29">
+      <c r="D6" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="23">
         <v>202</v>
       </c>
-      <c r="G6" s="28" t="s">
+      <c r="F6" s="23"/>
+      <c r="G6" s="22" t="s">
         <v>17</v>
       </c>
       <c r="I6" s="1"/>
@@ -917,16 +929,17 @@
       <c r="B7">
         <v>2969</v>
       </c>
-      <c r="C7" s="30">
+      <c r="C7" s="24">
         <v>43936</v>
       </c>
-      <c r="D7" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="29">
+      <c r="D7" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="23">
         <v>317</v>
       </c>
-      <c r="G7" s="28" t="s">
+      <c r="F7" s="23"/>
+      <c r="G7" s="22" t="s">
         <v>18</v>
       </c>
     </row>
@@ -934,16 +947,17 @@
       <c r="B8">
         <v>3121</v>
       </c>
-      <c r="C8" s="30">
+      <c r="C8" s="24">
         <v>43954</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="29">
+      <c r="E8" s="23">
         <v>307</v>
       </c>
-      <c r="G8" s="28" t="s">
+      <c r="F8" s="23"/>
+      <c r="G8" s="22" t="s">
         <v>20</v>
       </c>
       <c r="I8" s="1"/>
@@ -952,16 +966,19 @@
       <c r="B9">
         <v>3123</v>
       </c>
-      <c r="C9" s="30">
+      <c r="C9" s="24">
         <v>43955</v>
       </c>
-      <c r="D9" s="29" t="s">
+      <c r="D9" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="29">
+      <c r="E9" s="23">
         <v>305</v>
       </c>
-      <c r="G9" s="28" t="s">
+      <c r="F9" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="22" t="s">
         <v>22</v>
       </c>
     </row>
@@ -969,16 +986,17 @@
       <c r="B10">
         <v>3437</v>
       </c>
-      <c r="C10" s="30">
+      <c r="C10" s="24">
         <v>44103</v>
       </c>
-      <c r="D10" s="29" t="s">
+      <c r="D10" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="29">
+      <c r="E10" s="23">
         <v>319</v>
       </c>
-      <c r="G10" s="28" t="s">
+      <c r="F10" s="23"/>
+      <c r="G10" s="22" t="s">
         <v>24</v>
       </c>
       <c r="I10" s="1"/>
@@ -987,16 +1005,17 @@
       <c r="B11">
         <v>3687</v>
       </c>
-      <c r="C11" s="30">
+      <c r="C11" s="24">
         <v>44144</v>
       </c>
-      <c r="D11" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="29">
+      <c r="D11" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="23">
         <v>102</v>
       </c>
-      <c r="G11" s="28" t="s">
+      <c r="F11" s="23"/>
+      <c r="G11" s="22" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1004,16 +1023,17 @@
       <c r="B12">
         <v>3745</v>
       </c>
-      <c r="C12" s="30">
+      <c r="C12" s="24">
         <v>44152</v>
       </c>
-      <c r="D12" s="29" t="s">
+      <c r="D12" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="29">
+      <c r="E12" s="23">
         <v>336</v>
       </c>
-      <c r="G12" s="28" t="s">
+      <c r="F12" s="23"/>
+      <c r="G12" s="22" t="s">
         <v>27</v>
       </c>
       <c r="I12" s="1"/>
@@ -1022,16 +1042,17 @@
       <c r="B13">
         <v>3750</v>
       </c>
-      <c r="C13" s="30">
+      <c r="C13" s="24">
         <v>44158</v>
       </c>
-      <c r="D13" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="29">
+      <c r="D13" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="23">
         <v>117</v>
       </c>
-      <c r="G13" s="28" t="s">
+      <c r="F13" s="23"/>
+      <c r="G13" s="22" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1039,16 +1060,17 @@
       <c r="B14">
         <v>3763</v>
       </c>
-      <c r="C14" s="30">
+      <c r="C14" s="24">
         <v>44158</v>
       </c>
-      <c r="D14" s="29" t="s">
+      <c r="D14" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="29">
+      <c r="E14" s="23">
         <v>309</v>
       </c>
-      <c r="G14" s="28" t="s">
+      <c r="F14" s="23"/>
+      <c r="G14" s="22" t="s">
         <v>29</v>
       </c>
       <c r="I14" s="1"/>
@@ -1057,33 +1079,35 @@
       <c r="B15">
         <v>3787</v>
       </c>
-      <c r="C15" s="30">
+      <c r="C15" s="24">
         <v>44165</v>
       </c>
-      <c r="D15" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="29" t="s">
+      <c r="D15" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="G15" s="28" t="s">
-        <v>32</v>
+      <c r="F15" s="23"/>
+      <c r="G15" s="22" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>3795</v>
       </c>
-      <c r="C16" s="30">
+      <c r="C16" s="24">
         <v>44167</v>
       </c>
-      <c r="D16" s="29" t="s">
+      <c r="D16" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="29">
+      <c r="E16" s="23">
         <v>329</v>
       </c>
-      <c r="G16" s="28" t="s">
+      <c r="F16" s="23"/>
+      <c r="G16" s="22" t="s">
         <v>34</v>
       </c>
       <c r="I16" s="1"/>
@@ -1092,16 +1116,17 @@
       <c r="B17">
         <v>3914</v>
       </c>
-      <c r="C17" s="30">
+      <c r="C17" s="24">
         <v>44214</v>
       </c>
-      <c r="D17" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="29">
+      <c r="D17" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="23">
         <v>102</v>
       </c>
-      <c r="G17" s="28" t="s">
+      <c r="F17" s="23"/>
+      <c r="G17" s="22" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1109,16 +1134,17 @@
       <c r="B18">
         <v>3916</v>
       </c>
-      <c r="C18" s="30">
+      <c r="C18" s="24">
         <v>44214</v>
       </c>
-      <c r="D18" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="29">
+      <c r="D18" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="23">
         <v>137</v>
       </c>
-      <c r="G18" s="28" t="s">
+      <c r="F18" s="23"/>
+      <c r="G18" s="22" t="s">
         <v>36</v>
       </c>
       <c r="I18" s="1"/>
@@ -1127,33 +1153,37 @@
       <c r="B19">
         <v>3933</v>
       </c>
-      <c r="C19" s="30">
+      <c r="C19" s="24">
         <v>44214</v>
       </c>
-      <c r="D19" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="29">
+      <c r="D19" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="23">
         <v>307</v>
       </c>
-      <c r="G19" s="28" t="s">
-        <v>37</v>
+      <c r="F19" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="22" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>3937</v>
       </c>
-      <c r="C20" s="30">
+      <c r="C20" s="24">
         <v>44214</v>
       </c>
-      <c r="D20" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" s="29">
+      <c r="D20" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="23">
         <v>202</v>
       </c>
-      <c r="G20" s="28" t="s">
+      <c r="F20" s="23"/>
+      <c r="G20" s="22" t="s">
         <v>38</v>
       </c>
       <c r="I20" s="1"/>
@@ -1162,16 +1192,17 @@
       <c r="B21">
         <v>3959</v>
       </c>
-      <c r="C21" s="30">
+      <c r="C21" s="24">
         <v>44217</v>
       </c>
-      <c r="D21" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="29">
+      <c r="D21" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="23">
         <v>229</v>
       </c>
-      <c r="G21" s="28" t="s">
+      <c r="F21" s="23"/>
+      <c r="G21" s="22" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1179,16 +1210,19 @@
       <c r="B22">
         <v>3960</v>
       </c>
-      <c r="C22" s="30">
+      <c r="C22" s="24">
         <v>44217</v>
       </c>
-      <c r="D22" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" s="29">
+      <c r="D22" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="23">
         <v>307</v>
       </c>
-      <c r="G22" s="28" t="s">
+      <c r="F22" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" s="22" t="s">
         <v>39</v>
       </c>
       <c r="I22" s="1"/>
@@ -1197,16 +1231,19 @@
       <c r="B23">
         <v>3961</v>
       </c>
-      <c r="C23" s="30">
+      <c r="C23" s="24">
         <v>44217</v>
       </c>
-      <c r="D23" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="E23" s="29">
+      <c r="D23" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="23">
         <v>305</v>
       </c>
-      <c r="G23" s="28" t="s">
+      <c r="F23" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" s="22" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1214,16 +1251,19 @@
       <c r="B24">
         <v>3962</v>
       </c>
-      <c r="C24" s="30">
+      <c r="C24" s="24">
         <v>44217</v>
       </c>
-      <c r="D24" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" s="29">
+      <c r="D24" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="23">
         <v>303</v>
       </c>
-      <c r="G24" s="28" t="s">
+      <c r="F24" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" s="22" t="s">
         <v>41</v>
       </c>
       <c r="I24" s="1"/>
@@ -1232,16 +1272,17 @@
       <c r="B25">
         <v>3985</v>
       </c>
-      <c r="C25" s="30">
+      <c r="C25" s="24">
         <v>44225</v>
       </c>
-      <c r="D25" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" s="29">
+      <c r="D25" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="23">
         <v>111</v>
       </c>
-      <c r="G25" s="28" t="s">
+      <c r="F25" s="23"/>
+      <c r="G25" s="22" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1249,16 +1290,17 @@
       <c r="B26">
         <v>3986</v>
       </c>
-      <c r="C26" s="30">
+      <c r="C26" s="24">
         <v>44225</v>
       </c>
-      <c r="D26" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" s="29">
+      <c r="D26" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="23">
         <v>202</v>
       </c>
-      <c r="G26" s="28" t="s">
+      <c r="F26" s="23"/>
+      <c r="G26" s="22" t="s">
         <v>39</v>
       </c>
       <c r="I26" s="1"/>
@@ -1267,16 +1309,17 @@
       <c r="B27">
         <v>3987</v>
       </c>
-      <c r="C27" s="30">
+      <c r="C27" s="24">
         <v>44225</v>
       </c>
-      <c r="D27" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="E27" s="29">
+      <c r="D27" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="23">
         <v>211</v>
       </c>
-      <c r="G27" s="28" t="s">
+      <c r="F27" s="23"/>
+      <c r="G27" s="22" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1284,16 +1327,17 @@
       <c r="B28">
         <v>3988</v>
       </c>
-      <c r="C28" s="30">
+      <c r="C28" s="24">
         <v>44225</v>
       </c>
-      <c r="D28" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="E28" s="29">
+      <c r="D28" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="23">
         <v>222</v>
       </c>
-      <c r="G28" s="28" t="s">
+      <c r="F28" s="23"/>
+      <c r="G28" s="22" t="s">
         <v>39</v>
       </c>
       <c r="I28" s="1"/>
@@ -1302,33 +1346,35 @@
       <c r="B29">
         <v>3989</v>
       </c>
-      <c r="C29" s="30">
+      <c r="C29" s="24">
         <v>44225</v>
       </c>
-      <c r="D29" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="E29" s="29">
+      <c r="D29" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="23">
         <v>229</v>
       </c>
-      <c r="G29" s="28" t="s">
+      <c r="F29" s="23"/>
+      <c r="G29" s="22" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>3990</v>
       </c>
-      <c r="C30" s="30">
+      <c r="C30" s="24">
         <v>44225</v>
       </c>
-      <c r="D30" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="E30" s="29">
+      <c r="D30" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" s="23">
         <v>127</v>
       </c>
-      <c r="G30" s="28" t="s">
+      <c r="F30" s="23"/>
+      <c r="G30" s="22" t="s">
         <v>52</v>
       </c>
       <c r="I30" s="1"/>
@@ -1337,16 +1383,17 @@
       <c r="B31">
         <v>3990</v>
       </c>
-      <c r="C31" s="30">
+      <c r="C31" s="24">
         <v>44225</v>
       </c>
-      <c r="D31" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="E31" s="29">
+      <c r="D31" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" s="23">
         <v>127</v>
       </c>
-      <c r="G31" s="28" t="s">
+      <c r="F31" s="23"/>
+      <c r="G31" s="22" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1354,16 +1401,17 @@
       <c r="B32">
         <v>3991</v>
       </c>
-      <c r="C32" s="30">
+      <c r="C32" s="24">
         <v>44225</v>
       </c>
-      <c r="D32" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="E32" s="29">
+      <c r="D32" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="23">
         <v>218</v>
       </c>
-      <c r="G32" s="28" t="s">
+      <c r="F32" s="23"/>
+      <c r="G32" s="22" t="s">
         <v>55</v>
       </c>
       <c r="I32" s="1"/>
@@ -1372,16 +1420,19 @@
       <c r="B33">
         <v>3993</v>
       </c>
-      <c r="C33" s="30">
+      <c r="C33" s="24">
         <v>44225</v>
       </c>
-      <c r="D33" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="E33" s="29">
+      <c r="D33" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" s="23">
         <v>303</v>
       </c>
-      <c r="G33" s="28" t="s">
+      <c r="F33" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="G33" s="22" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1389,16 +1440,19 @@
       <c r="B34">
         <v>3993</v>
       </c>
-      <c r="C34" s="30">
+      <c r="C34" s="24">
         <v>44225</v>
       </c>
-      <c r="D34" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="E34" s="29">
+      <c r="D34" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" s="23">
         <v>303</v>
       </c>
-      <c r="G34" s="28" t="s">
+      <c r="F34" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="G34" s="22" t="s">
         <v>43</v>
       </c>
       <c r="I34" s="1"/>
@@ -1407,16 +1461,17 @@
       <c r="B35">
         <v>4050</v>
       </c>
-      <c r="C35" s="30">
+      <c r="C35" s="24">
         <v>44237</v>
       </c>
-      <c r="D35" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="E35" s="29">
+      <c r="D35" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" s="23">
         <v>224</v>
       </c>
-      <c r="G35" s="28" t="s">
+      <c r="F35" s="23"/>
+      <c r="G35" s="22" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1424,16 +1479,17 @@
       <c r="B36">
         <v>4050</v>
       </c>
-      <c r="C36" s="30">
+      <c r="C36" s="24">
         <v>44237</v>
       </c>
-      <c r="D36" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="E36" s="29">
+      <c r="D36" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" s="23">
         <v>224</v>
       </c>
-      <c r="G36" s="28" t="s">
+      <c r="F36" s="23"/>
+      <c r="G36" s="22" t="s">
         <v>45</v>
       </c>
       <c r="I36" s="1"/>
@@ -1442,16 +1498,17 @@
       <c r="B37">
         <v>4050</v>
       </c>
-      <c r="C37" s="30">
+      <c r="C37" s="24">
         <v>44237</v>
       </c>
-      <c r="D37" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="E37" s="29">
+      <c r="D37" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E37" s="23">
         <v>224</v>
       </c>
-      <c r="G37" s="28" t="s">
+      <c r="F37" s="23"/>
+      <c r="G37" s="22" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1459,16 +1516,17 @@
       <c r="B38">
         <v>4054</v>
       </c>
-      <c r="C38" s="30">
+      <c r="C38" s="24">
         <v>44238</v>
       </c>
-      <c r="D38" s="29" t="s">
+      <c r="D38" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="E38" s="29">
+      <c r="E38" s="23">
         <v>111</v>
       </c>
-      <c r="G38" s="28" t="s">
+      <c r="F38" s="23"/>
+      <c r="G38" s="22" t="s">
         <v>48</v>
       </c>
       <c r="I38" s="1"/>
@@ -1477,16 +1535,17 @@
       <c r="B39">
         <v>4055</v>
       </c>
-      <c r="C39" s="30">
+      <c r="C39" s="24">
         <v>44238</v>
       </c>
-      <c r="D39" s="29" t="s">
+      <c r="D39" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="E39" s="29">
+      <c r="E39" s="23">
         <v>110</v>
       </c>
-      <c r="G39" s="28" t="s">
+      <c r="F39" s="23"/>
+      <c r="G39" s="22" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1494,16 +1553,17 @@
       <c r="B40">
         <v>4056</v>
       </c>
-      <c r="C40" s="30">
+      <c r="C40" s="24">
         <v>44238</v>
       </c>
-      <c r="D40" s="29" t="s">
+      <c r="D40" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="E40" s="29">
+      <c r="E40" s="23">
         <v>122</v>
       </c>
-      <c r="G40" s="28" t="s">
+      <c r="F40" s="23"/>
+      <c r="G40" s="22" t="s">
         <v>50</v>
       </c>
       <c r="I40" s="1"/>
@@ -1512,16 +1572,17 @@
       <c r="B41">
         <v>4071</v>
       </c>
-      <c r="C41" s="30">
+      <c r="C41" s="24">
         <v>44242</v>
       </c>
-      <c r="D41" s="29" t="s">
+      <c r="D41" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="E41" s="29">
+      <c r="E41" s="23">
         <v>102</v>
       </c>
-      <c r="G41" s="28" t="s">
+      <c r="F41" s="23"/>
+      <c r="G41" s="22" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1529,16 +1590,17 @@
       <c r="B42">
         <v>4074</v>
       </c>
-      <c r="C42" s="30">
+      <c r="C42" s="24">
         <v>44242</v>
       </c>
-      <c r="D42" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="E42" s="29" t="s">
+      <c r="D42" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E42" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="G42" s="28" t="s">
+      <c r="F42" s="23"/>
+      <c r="G42" s="22" t="s">
         <v>51</v>
       </c>
       <c r="I42" s="1"/>
@@ -1556,7 +1618,7 @@
   <dimension ref="B1:J39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B39" sqref="B2:G39"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1841,7 +1903,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="7">
         <v>3787</v>
       </c>
@@ -2247,204 +2309,204 @@
       <c r="J26" s="11"/>
     </row>
     <row r="27" spans="2:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="26">
+      <c r="B27" s="20">
         <v>3990</v>
       </c>
-      <c r="C27" s="27">
+      <c r="C27" s="21">
         <v>44225</v>
       </c>
-      <c r="D27" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="E27" s="21">
+      <c r="D27" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="15">
         <v>127</v>
       </c>
-      <c r="F27" s="21">
+      <c r="F27" s="15">
         <v>1</v>
       </c>
       <c r="G27" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="H27" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="I27" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="J27" s="23"/>
+      <c r="H27" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I27" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J27" s="17"/>
     </row>
     <row r="28" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="26">
+      <c r="B28" s="20">
         <v>3990</v>
       </c>
-      <c r="C28" s="27">
+      <c r="C28" s="21">
         <v>44225</v>
       </c>
-      <c r="D28" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="E28" s="21">
+      <c r="D28" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="15">
         <v>127</v>
       </c>
-      <c r="F28" s="21">
+      <c r="F28" s="15">
         <v>1</v>
       </c>
       <c r="G28" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="25"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="19">
+      <c r="B29" s="13">
         <v>3991</v>
       </c>
-      <c r="C29" s="20">
+      <c r="C29" s="14">
         <v>44225</v>
       </c>
-      <c r="D29" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="E29" s="22">
+      <c r="D29" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="16">
         <v>218</v>
       </c>
-      <c r="F29" s="22">
+      <c r="F29" s="16">
         <v>2</v>
       </c>
       <c r="G29" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="H29" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="I29" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="J29" s="23"/>
+      <c r="H29" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="I29" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="J29" s="17"/>
     </row>
     <row r="30" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="26">
+      <c r="B30" s="20">
         <v>3993</v>
       </c>
-      <c r="C30" s="27">
+      <c r="C30" s="21">
         <v>44225</v>
       </c>
-      <c r="D30" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="E30" s="21">
+      <c r="D30" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" s="15">
         <v>303</v>
       </c>
-      <c r="F30" s="21">
+      <c r="F30" s="15">
         <v>3</v>
       </c>
       <c r="G30" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="H30" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="I30" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="J30" s="16"/>
+      <c r="H30" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I30" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J30" s="25"/>
     </row>
     <row r="31" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="26">
+      <c r="B31" s="20">
         <v>3993</v>
       </c>
-      <c r="C31" s="27">
+      <c r="C31" s="21">
         <v>44225</v>
       </c>
-      <c r="D31" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="E31" s="21">
+      <c r="D31" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" s="15">
         <v>303</v>
       </c>
-      <c r="F31" s="21">
+      <c r="F31" s="15">
         <v>3</v>
       </c>
       <c r="G31" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="H31" s="24"/>
-      <c r="I31" s="24"/>
-      <c r="J31" s="17"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="26"/>
     </row>
     <row r="32" spans="2:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="26">
+      <c r="B32" s="20">
         <v>4050</v>
       </c>
-      <c r="C32" s="27">
+      <c r="C32" s="21">
         <v>44237</v>
       </c>
-      <c r="D32" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="E32" s="21">
+      <c r="D32" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="15">
         <v>224</v>
       </c>
-      <c r="F32" s="21">
+      <c r="F32" s="15">
         <v>2</v>
       </c>
       <c r="G32" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="H32" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="I32" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="J32" s="16"/>
+      <c r="H32" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="I32" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="J32" s="25"/>
     </row>
     <row r="33" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="26">
+      <c r="B33" s="20">
         <v>4050</v>
       </c>
-      <c r="C33" s="27">
+      <c r="C33" s="21">
         <v>44237</v>
       </c>
-      <c r="D33" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="E33" s="21">
+      <c r="D33" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" s="15">
         <v>224</v>
       </c>
-      <c r="F33" s="21">
+      <c r="F33" s="15">
         <v>2</v>
       </c>
       <c r="G33" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="H33" s="14"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="17"/>
+      <c r="H33" s="28"/>
+      <c r="I33" s="28"/>
+      <c r="J33" s="26"/>
     </row>
     <row r="34" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="26">
+      <c r="B34" s="20">
         <v>4050</v>
       </c>
-      <c r="C34" s="27">
+      <c r="C34" s="21">
         <v>44237</v>
       </c>
-      <c r="D34" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="E34" s="21">
+      <c r="D34" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" s="15">
         <v>224</v>
       </c>
-      <c r="F34" s="21">
+      <c r="F34" s="15">
         <v>2</v>
       </c>
       <c r="G34" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="H34" s="15"/>
-      <c r="I34" s="15"/>
-      <c r="J34" s="18"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="29"/>
+      <c r="J34" s="30"/>
     </row>
     <row r="35" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="7">

</xml_diff>